<commit_message>
updated cases and addded list of temple sites
</commit_message>
<xml_diff>
--- a/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
+++ b/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Janak_Jain/Janak/Personal/projects/hindus_in_pakistan/github/hindus_in_pakistan/data/daahip-w/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C4F568-4816-A240-BD20-88608CF5D66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4703E77F-15EE-5C48-9D90-9EC663053995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{7834C0CA-90C6-1E41-85BA-104BC8C7D625}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" xr2:uid="{7834C0CA-90C6-1E41-85BA-104BC8C7D625}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="492">
   <si>
     <t>city</t>
   </si>
@@ -1571,6 +1571,69 @@
   <si>
     <t>https://twitter.com/NarainDasBheel8/status/1612031515785072643?s=20&amp;t=37g10exefm4l7cU-JhUmkg
 https://twitter.com/voice_minority/status/1347411421932494851?s=20&amp;t=Z5hu76J6UO7-KqG7vnfo7A</t>
+  </si>
+  <si>
+    <t>case_65</t>
+  </si>
+  <si>
+    <t>Karishma</t>
+  </si>
+  <si>
+    <t>d/o Ramesh Bheel</t>
+  </si>
+  <si>
+    <t>Naukot</t>
+  </si>
+  <si>
+    <t>Kanwal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peer Ayoub Jaan Sarhandi </t>
+  </si>
+  <si>
+    <t>Naukot Mirpurkhas Sindh:
+18-2-2023 A minor Hindu girl Karishma d/o Ramesh Bheel, has been converted to Islam at gargha of peer Ayoub Jaan Sarhandi and became Kanwal, and now she will be married to the kidnapper.</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1627272301275234304</t>
+  </si>
+  <si>
+    <t>case_66</t>
+  </si>
+  <si>
+    <t>Sohbatpur</t>
+  </si>
+  <si>
+    <t>Jaffarabad</t>
+  </si>
+  <si>
+    <t>Kumari d/o Bhag Chand</t>
+  </si>
+  <si>
+    <t>Aisha</t>
+  </si>
+  <si>
+    <t>Bibi</t>
+  </si>
+  <si>
+    <t>Amir Nawaz s/o Ali Nawaz</t>
+  </si>
+  <si>
+    <t>53501-0341993-5</t>
+  </si>
+  <si>
+    <t>53201-4229617-6</t>
+  </si>
+  <si>
+    <t>Another Pak Hindu minor girl Kanwal kumari abducted, converted to Islam &amp; forced into Nikah sl@very by abductor Amir Nawaz. Her Muslim name is Aisha Bibi. Another addition to statistics.
+Pakistan on ethnic cleansing spree of Hindus. Does anyone care?
+Source: Pak Hindu activists</t>
+  </si>
+  <si>
+    <t>https://twitter.com/pakistan_untold/status/1639300494245130242</t>
+  </si>
+  <si>
+    <t>Pakistan Untold</t>
   </si>
 </sst>
 </file>
@@ -1967,12 +2030,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}">
-  <dimension ref="A1:AL65"/>
+  <dimension ref="A1:AL67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3067,7 +3130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>146</v>
       </c>
@@ -3490,7 +3553,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="238" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" ht="221" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>185</v>
       </c>
@@ -6073,6 +6136,145 @@
       </c>
       <c r="AL65" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>472</v>
+      </c>
+      <c r="B66" t="s">
+        <v>475</v>
+      </c>
+      <c r="C66" t="s">
+        <v>84</v>
+      </c>
+      <c r="D66" t="s">
+        <v>36</v>
+      </c>
+      <c r="E66">
+        <v>24.854103363133799</v>
+      </c>
+      <c r="F66">
+        <v>69.403801880405993</v>
+      </c>
+      <c r="G66" s="2">
+        <v>44975</v>
+      </c>
+      <c r="I66" t="s">
+        <v>473</v>
+      </c>
+      <c r="J66" t="s">
+        <v>474</v>
+      </c>
+      <c r="K66" t="s">
+        <v>476</v>
+      </c>
+      <c r="N66">
+        <v>19</v>
+      </c>
+      <c r="P66" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>171</v>
+      </c>
+      <c r="R66" t="b">
+        <v>1</v>
+      </c>
+      <c r="T66" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA66" t="s">
+        <v>477</v>
+      </c>
+      <c r="AC66" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD66" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH66" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="AI66" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ66" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="AL66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:38" ht="170" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>480</v>
+      </c>
+      <c r="B67" t="s">
+        <v>481</v>
+      </c>
+      <c r="C67" t="s">
+        <v>482</v>
+      </c>
+      <c r="D67" t="s">
+        <v>176</v>
+      </c>
+      <c r="E67">
+        <v>28.517991037086102</v>
+      </c>
+      <c r="F67">
+        <v>68.543819106223594</v>
+      </c>
+      <c r="G67" s="2">
+        <v>43880</v>
+      </c>
+      <c r="H67" t="s">
+        <v>488</v>
+      </c>
+      <c r="I67" t="s">
+        <v>476</v>
+      </c>
+      <c r="J67" t="s">
+        <v>483</v>
+      </c>
+      <c r="K67" t="s">
+        <v>484</v>
+      </c>
+      <c r="L67" t="s">
+        <v>485</v>
+      </c>
+      <c r="P67" t="s">
+        <v>148</v>
+      </c>
+      <c r="R67" t="b">
+        <v>1</v>
+      </c>
+      <c r="T67" t="b">
+        <v>1</v>
+      </c>
+      <c r="W67" t="s">
+        <v>486</v>
+      </c>
+      <c r="X67" t="s">
+        <v>487</v>
+      </c>
+      <c r="Y67" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD67" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH67" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="AI67" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ67" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="AL67" t="s">
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -6161,6 +6363,8 @@
     <hyperlink ref="AJ63" r:id="rId81" xr:uid="{6251C1C3-FA6F-9647-A588-734760DE1FFA}"/>
     <hyperlink ref="AJ64" r:id="rId82" xr:uid="{D0821144-3AAE-034A-BFB2-18846C0A7AD9}"/>
     <hyperlink ref="AJ65" r:id="rId83" xr:uid="{5BACCFC3-3E71-7440-926C-B6580C9AA540}"/>
+    <hyperlink ref="AJ66" r:id="rId84" xr:uid="{A7FC2155-852B-E34D-8C7A-1747F199DEF3}"/>
+    <hyperlink ref="AJ67" r:id="rId85" xr:uid="{E438BF62-D038-9A4B-9903-FE3E0C247D62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
added 20 new cases
</commit_message>
<xml_diff>
--- a/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
+++ b/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Janak_Jain/Janak/Personal/projects/hindus_in_pakistan/github/hindus_in_pakistan/data/daahip-w/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D9668B-C0FF-474F-8A20-50913440E403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554D09CA-50E6-EE4F-9A77-352F6E720975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{7834C0CA-90C6-1E41-85BA-104BC8C7D625}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="cases" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cases!$A$1:$AL$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cases!$A$1:$AL$93</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="671">
   <si>
     <t>city</t>
   </si>
@@ -1798,12 +1798,470 @@
   <si>
     <t>Matiari</t>
   </si>
+  <si>
+    <t>case_74</t>
+  </si>
+  <si>
+    <t>Tharparkar Sindh:
+Abducted Hindu minor girl, Leelan d/o Karamchand Meghwar of Kankio village, converted to Islam and married Niaz Ahmad.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1663950417099907072</t>
+  </si>
+  <si>
+    <t>Leelan d/o Karamchand</t>
+  </si>
+  <si>
+    <t>Kantio</t>
+  </si>
+  <si>
+    <t>Niaz Ahmed</t>
+  </si>
+  <si>
+    <t>case_75</t>
+  </si>
+  <si>
+    <t>Ghotki</t>
+  </si>
+  <si>
+    <t>Zarina</t>
+  </si>
+  <si>
+    <t>Killing</t>
+  </si>
+  <si>
+    <t>Ghotki Sindh;
+The horrifying and heart-wrenching incident in Ghotki! A brave Hindu woman, #Zarina_Bheel, was killed while defending her daughter from abduction. It's appalling that justice is yet to be served, and the accused must be held accountable for their heinous act</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1662774102535331840</t>
+  </si>
+  <si>
+    <t>Killed while trying to avoid abduction of her daughter</t>
+  </si>
+  <si>
+    <t>case_76</t>
+  </si>
+  <si>
+    <t>Daharki</t>
+  </si>
+  <si>
+    <t>Dharki, Sindh
+A married Hindu woman, Sangeeta Oad, has been converted and married at Bharchundi Dargha of Mian Javeed Ahemd Qadri; her abductor's name has not been revealed.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1661212480046080001</t>
+  </si>
+  <si>
+    <t>Sangeeta</t>
+  </si>
+  <si>
+    <t>Oad</t>
+  </si>
+  <si>
+    <t>case_77</t>
+  </si>
+  <si>
+    <t>Pithoro,Umarkot Sindh
+A Hindu girl Hasena Oad has been abducted by Shokat shar and 4 others by gun point,father of girl filed complaint at police station against 5 accused belonging to the Shar community.Girl will forcibly married to shokat shar father told
+#StopForcedConversions</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1659524774811299841</t>
+  </si>
+  <si>
+    <t>Haseena</t>
+  </si>
+  <si>
+    <t>Shokat Shar</t>
+  </si>
+  <si>
+    <t>case_78</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1659249097818112007</t>
+  </si>
+  <si>
+    <t>Badin Sindh:
+A minor Hindu girl Tooti d/o Babu Maheshwari, a resident of Kareo Ghanwar Gharibabad, was abducted a few days ago now she has been converted to Islam and married to Fida Hussain Khaskheli.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>Kario Ghanwar</t>
+  </si>
+  <si>
+    <t>Tooti d/o Babu</t>
+  </si>
+  <si>
+    <t>Fida Hussain Khaskheli</t>
+  </si>
+  <si>
+    <t>case_79</t>
+  </si>
+  <si>
+    <t>Mirpurkhas Sindh:
+Dharmi Bheel, a married woman of Mirpurkhas phuladio was abducted and married to Muslim Mir Muhammad Shar after converting the religion in Pir Ayub Jan Sirhandi Samaro.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1658537910491045896</t>
+  </si>
+  <si>
+    <t>Mir Muhammad Shar</t>
+  </si>
+  <si>
+    <t>Pir Ayub Jan Sirhandi</t>
+  </si>
+  <si>
+    <t>Dharmi</t>
+  </si>
+  <si>
+    <t>Phuladio</t>
+  </si>
+  <si>
+    <t>case_80</t>
+  </si>
+  <si>
+    <t>Karachi Haji Mureed Village Goli Mar Chowrangi</t>
+  </si>
+  <si>
+    <t>w/o Ramji Meghwar</t>
+  </si>
+  <si>
+    <t>44103-5532996-6</t>
+  </si>
+  <si>
+    <t>Rida Bai</t>
+  </si>
+  <si>
+    <t>Resident of Mohallah Sattar Nagar D.B.P. Mirpur Khan</t>
+  </si>
+  <si>
+    <t>case_81</t>
+  </si>
+  <si>
+    <t>Meeran</t>
+  </si>
+  <si>
+    <t>d/o Ramji Meghwar</t>
+  </si>
+  <si>
+    <t>Karachi Sindh:
+It is very sad to say that what is happening every day, Karachi Haji Mureed Village Goli Mar Chowrangi, since 7-05-2023 the whole family of #Ramji_Meghwar is missing, he is worried and tired from the police station for a week. No response yet.....</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1657429814377168898</t>
+  </si>
+  <si>
+    <t>few days ago we highlighted the case of a Hindu family kidnapped from Karachi. Now it is heard that they have converted.Why are Hindus attacked,Specially,Sindh province has more cases of religious conversion.
+Meeran 14y,Priya 12y ,Sanju 11y, Amarlal 9y,Jairam,Gopal, are included.</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1658409406365589505</t>
+  </si>
+  <si>
+    <t>case_82</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Linked to case 80</t>
+  </si>
+  <si>
+    <t>case_83</t>
+  </si>
+  <si>
+    <t>Pooja Kumari</t>
+  </si>
+  <si>
+    <t>d/o Kanhaiya Lal Meghwar</t>
+  </si>
+  <si>
+    <t>Sanghar Sindh:
+Pooja kumari d/o khaniya Kal meghwar, With victims of force conversion at High Court of Sindh at Hyderabad, their Daughter has been forcefully abducted and converted to Islam.
+ #StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1657076074453549057</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1655466135523827712</t>
+  </si>
+  <si>
+    <t>Kotari Hyderabad Sindh:
+Hindu girl Meena Kumari, d/o  Mangal das Meghwar, who was abducted three days ago from Kotari, Sindh has not yet been recovered.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>case_84</t>
+  </si>
+  <si>
+    <t>Kotri</t>
+  </si>
+  <si>
+    <t>Jamshoro</t>
+  </si>
+  <si>
+    <t>Meena Kumari</t>
+  </si>
+  <si>
+    <t>d/o  Mangal das Meghwar</t>
+  </si>
+  <si>
+    <t>Muzamil Mianwali</t>
+  </si>
+  <si>
+    <t>case_85</t>
+  </si>
+  <si>
+    <t>Karachi Sindh:
+Now that daily killings and cruelty have become a daily routine for Hindus, at night again, an innocent A Hindu girl Jiya Hari Maheshwari, was kidnapped by Muzamil Mianwali from Dariyaabad area of ​​Lyari.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1654548585730527232</t>
+  </si>
+  <si>
+    <t>Jiya</t>
+  </si>
+  <si>
+    <t>d/o Hari Maheshwari</t>
+  </si>
+  <si>
+    <t>Daryabad</t>
+  </si>
+  <si>
+    <t>case_86</t>
+  </si>
+  <si>
+    <t>Devi</t>
+  </si>
+  <si>
+    <t>Dino Bheel</t>
+  </si>
+  <si>
+    <t>Deharki Sindh:
+27 April A Hindu girl Devi d/o Dino Bheel abducted from Dehrki Sindh, converted in Rahim Yar Khan was married to Muhammed Ali, a resident of Punjab.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1654357488693571584</t>
+  </si>
+  <si>
+    <t>Misbah</t>
+  </si>
+  <si>
+    <t>Talha Umar</t>
+  </si>
+  <si>
+    <t>435030530295-3</t>
+  </si>
+  <si>
+    <t>case_87</t>
+  </si>
+  <si>
+    <t>Mirpurkhas Sindh:
+A minor Hindu Ggirl Lachmi d/o Pahalwan Bhaat resident of sindhri, Sindh has been converted to Islam by Molvi Munir Ahmed of Rahim yar khan Punjab and married of to Imtiaz Ali. Lachmi became Aisha Bibi.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1653979445567590404</t>
+  </si>
+  <si>
+    <t>d/o Pahalwan Bhaat</t>
+  </si>
+  <si>
+    <t>Sindhre</t>
+  </si>
+  <si>
+    <t>Munir Ahmed</t>
+  </si>
+  <si>
+    <t>Rahim Yar Khan, Punjab</t>
+  </si>
+  <si>
+    <t>Imtiaz Ali</t>
+  </si>
+  <si>
+    <t>Bhaat</t>
+  </si>
+  <si>
+    <t>case_88</t>
+  </si>
+  <si>
+    <t>Umerkot Samaro Sindh:
+The 16-year-old Hindu girl Hina Maharaj d/o Kasturo Maharaj, was abducted and converted and married  to Gulam Mustafa Brohi.
+#StopForcedConversions
+#HinduLivesMatters</t>
+  </si>
+  <si>
+    <t>Maharaj</t>
+  </si>
+  <si>
+    <t>d/o Kasturo Maharaj</t>
+  </si>
+  <si>
+    <t>Gulam Mustafa Brohi</t>
+  </si>
+  <si>
+    <t>Fatema</t>
+  </si>
+  <si>
+    <t>case_89</t>
+  </si>
+  <si>
+    <t>Sanghar sindh:
+Another married Hindu girl Ganga d/o Chetan bheel from Jhole twon was abducted 3 days ago and converted to Islam.
+Petition has been filed in court.
+#StopForcedConversions
+#HinduLivesMatters</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1653319169138479108</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1653076299307528192</t>
+  </si>
+  <si>
+    <t>Ganga</t>
+  </si>
+  <si>
+    <t>d/o Chetan bheel</t>
+  </si>
+  <si>
+    <t>Jhol</t>
+  </si>
+  <si>
+    <t>case_90</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1653032129486266368</t>
+  </si>
+  <si>
+    <t>Karachi Sindh:
+A minor Hindu girl Pars d/o Morji Maheshwari, a minor Sindhi Hindu daughter of the resident of Ghulam Shah Lane Lyari, was kidnapped 15 days ago. Now the daughter has changed her religion and got married. We appeal to the higher authorities to return our daughter.</t>
+  </si>
+  <si>
+    <t>Ghulam Shah Lane, Lyari</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>d/o Moorjee Maheshwari</t>
+  </si>
+  <si>
+    <t>New Dambalu, Tando Ghulam Ali Sindh:
+The Hindu girl Resham Kolhi has been converted to Islam at Pir Ayub Jan Sirhandi. Resham became Ayesha, and married off to Shah Nawaz Dars, a resident of New Dambalu.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1652938928087859202</t>
+  </si>
+  <si>
+    <t>case_91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Dambalu, Tando Ghulam Ali </t>
+  </si>
+  <si>
+    <t>Resham</t>
+  </si>
+  <si>
+    <t>Shaikh</t>
+  </si>
+  <si>
+    <t>d/o Pardesi Kolhi</t>
+  </si>
+  <si>
+    <t>Shahnawaz s/o Jani Dars</t>
+  </si>
+  <si>
+    <t>41103-5869377-5</t>
+  </si>
+  <si>
+    <t>case_92</t>
+  </si>
+  <si>
+    <t>Mithi Tharparkar Sindh:
+Minor girl Gudi Kolhi and her parents are being pressured by the criminals to hand over the Gudi to the criminals. Sindh government and human rights institutions should take action and save this minority girl as much as possible.
+#StopForcedConversions</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1651469763472932870</t>
+  </si>
+  <si>
+    <t>Gudi</t>
+  </si>
+  <si>
+    <t>Harassment</t>
+  </si>
+  <si>
+    <t>case_93</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1651202209487388674</t>
+  </si>
+  <si>
+    <t>Khanpur Maher Sindh 
+The minor Hindu girl Payal who was recovered from Karachi after being abducted from Khanpur Mehar appeared before the magistrate girl has given a statement in the court that she wants to go with her parents.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>Khanpur Mahar</t>
+  </si>
+  <si>
+    <t>Payal Kumari</t>
+  </si>
+  <si>
+    <t>Theft</t>
+  </si>
+  <si>
+    <t>case_94</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1649092599050031105</t>
+  </si>
+  <si>
+    <t>Jhol Sanghar Sindh
+A Hindu girl who converted to Islam about 4 months ago became Hassina.
+Now her husband Azmat Mari divorced her on the advice of influential people.
+He left her parents home.
+#StopForcedConversions
+#saveminoritygirls</t>
+  </si>
+  <si>
+    <t>Hassina</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Abandonment</t>
+  </si>
+  <si>
+    <t>Azmat Mari</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1823,6 +2281,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1864,7 +2329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1878,6 +2343,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2193,17 +2659,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}">
-  <dimension ref="A1:AL74"/>
+  <dimension ref="A1:AL95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="68.5" customWidth="1"/>
     <col min="36" max="36" width="40.1640625" customWidth="1"/>
   </cols>
@@ -2324,7 +2791,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -2410,7 +2877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -2478,7 +2945,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -2531,7 +2998,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -2575,7 +3042,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -2646,7 +3113,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -2693,7 +3160,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="187" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -2752,7 +3219,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -2805,7 +3272,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -2876,7 +3343,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>105</v>
       </c>
@@ -2938,7 +3405,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -3012,7 +3479,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3086,7 +3553,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="170" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3151,7 +3618,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>125</v>
       </c>
@@ -3216,7 +3683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -3293,7 +3760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" ht="323" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>146</v>
       </c>
@@ -3376,7 +3843,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="255" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:38" ht="187" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>150</v>
       </c>
@@ -3453,7 +3920,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="85" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -3512,7 +3979,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="204" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38" ht="136" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>160</v>
       </c>
@@ -3586,7 +4053,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>169</v>
       </c>
@@ -3716,7 +4183,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="221" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" ht="153" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>185</v>
       </c>
@@ -3781,7 +4248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -3843,7 +4310,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>199</v>
       </c>
@@ -3905,7 +4372,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>203</v>
       </c>
@@ -3991,7 +4458,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>211</v>
       </c>
@@ -4056,7 +4523,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:38" ht="153" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>216</v>
       </c>
@@ -4115,7 +4582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>228</v>
       </c>
@@ -4198,7 +4665,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:38" ht="187" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:38" ht="170" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>235</v>
       </c>
@@ -4272,7 +4739,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:38" ht="153" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38" ht="136" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>243</v>
       </c>
@@ -4337,7 +4804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>251</v>
       </c>
@@ -4393,7 +4860,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>256</v>
       </c>
@@ -4912,7 +5379,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="42" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>293</v>
       </c>
@@ -4971,7 +5438,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>298</v>
       </c>
@@ -5083,7 +5550,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>308</v>
       </c>
@@ -5139,7 +5606,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>313</v>
       </c>
@@ -5207,7 +5674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:38" ht="153" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>331</v>
       </c>
@@ -5281,7 +5748,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:38" ht="170" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>334</v>
       </c>
@@ -5426,7 +5893,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>341</v>
       </c>
@@ -5500,7 +5967,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>344</v>
       </c>
@@ -5565,7 +6032,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:38" ht="153" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>352</v>
       </c>
@@ -5692,7 +6159,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>372</v>
       </c>
@@ -5751,7 +6218,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>375</v>
       </c>
@@ -5869,7 +6336,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>386</v>
       </c>
@@ -5986,7 +6453,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:38" ht="136" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>420</v>
       </c>
@@ -6042,7 +6509,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>424</v>
       </c>
@@ -6092,7 +6559,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:38" ht="51" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:38" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>429</v>
       </c>
@@ -6139,7 +6606,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>453</v>
       </c>
@@ -6192,7 +6659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:38" ht="68" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:38" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>458</v>
       </c>
@@ -6245,7 +6712,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:38" ht="119" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:38" ht="102" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>461</v>
       </c>
@@ -6301,7 +6768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:38" ht="68" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>472</v>
       </c>
@@ -6369,7 +6836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:38" ht="170" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:38" ht="119" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>480</v>
       </c>
@@ -6440,7 +6907,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="68" spans="1:38" ht="153" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:38" ht="85" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>492</v>
       </c>
@@ -6508,7 +6975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:38" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:38" ht="306" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>497</v>
       </c>
@@ -6591,7 +7058,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:38" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:38" ht="356" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>504</v>
       </c>
@@ -6671,7 +7138,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:38" ht="289" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:38" ht="238" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>515</v>
       </c>
@@ -6883,8 +7350,1355 @@
         <v>24</v>
       </c>
     </row>
+    <row r="75" spans="1:38" ht="85" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>536</v>
+      </c>
+      <c r="B75" t="s">
+        <v>540</v>
+      </c>
+      <c r="C75" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" t="s">
+        <v>36</v>
+      </c>
+      <c r="E75">
+        <v>25.1725001479894</v>
+      </c>
+      <c r="F75">
+        <v>69.9697921381387</v>
+      </c>
+      <c r="G75" s="2">
+        <v>45077</v>
+      </c>
+      <c r="I75" t="s">
+        <v>539</v>
+      </c>
+      <c r="J75" t="s">
+        <v>33</v>
+      </c>
+      <c r="O75" t="s">
+        <v>33</v>
+      </c>
+      <c r="P75" t="s">
+        <v>148</v>
+      </c>
+      <c r="T75" t="b">
+        <v>1</v>
+      </c>
+      <c r="W75" t="s">
+        <v>541</v>
+      </c>
+      <c r="Y75" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB75" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD75" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH75" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="AI75" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ75" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="AL75" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:38" ht="85" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>542</v>
+      </c>
+      <c r="B76" t="s">
+        <v>543</v>
+      </c>
+      <c r="C76" t="s">
+        <v>543</v>
+      </c>
+      <c r="D76" t="s">
+        <v>36</v>
+      </c>
+      <c r="E76">
+        <v>28.027125086794001</v>
+      </c>
+      <c r="F76">
+        <v>69.326548803422796</v>
+      </c>
+      <c r="G76" s="2">
+        <v>45074</v>
+      </c>
+      <c r="I76" t="s">
+        <v>544</v>
+      </c>
+      <c r="J76" t="s">
+        <v>75</v>
+      </c>
+      <c r="O76" t="s">
+        <v>75</v>
+      </c>
+      <c r="P76" t="s">
+        <v>545</v>
+      </c>
+      <c r="T76" t="b">
+        <v>0</v>
+      </c>
+      <c r="V76" t="s">
+        <v>548</v>
+      </c>
+      <c r="AH76" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="AI76" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ76" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="AL76" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>549</v>
+      </c>
+      <c r="B77" t="s">
+        <v>550</v>
+      </c>
+      <c r="C77" t="s">
+        <v>543</v>
+      </c>
+      <c r="D77" t="s">
+        <v>36</v>
+      </c>
+      <c r="E77">
+        <v>28.0400028999934</v>
+      </c>
+      <c r="F77">
+        <v>69.681262299376399</v>
+      </c>
+      <c r="G77" s="2">
+        <v>45069</v>
+      </c>
+      <c r="I77" t="s">
+        <v>553</v>
+      </c>
+      <c r="J77" t="s">
+        <v>554</v>
+      </c>
+      <c r="O77" t="s">
+        <v>554</v>
+      </c>
+      <c r="P77" t="s">
+        <v>148</v>
+      </c>
+      <c r="T77" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y77" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA77" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB77" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC77" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD77" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH77" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="AI77" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ77" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="AL77" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:38" ht="85" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>555</v>
+      </c>
+      <c r="B78" t="s">
+        <v>339</v>
+      </c>
+      <c r="C78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D78" t="s">
+        <v>36</v>
+      </c>
+      <c r="E78">
+        <v>25.5107279994685</v>
+      </c>
+      <c r="F78">
+        <v>69.375502379351104</v>
+      </c>
+      <c r="G78" s="2">
+        <v>45065</v>
+      </c>
+      <c r="I78" t="s">
+        <v>558</v>
+      </c>
+      <c r="J78" t="s">
+        <v>554</v>
+      </c>
+      <c r="O78" t="s">
+        <v>554</v>
+      </c>
+      <c r="P78" t="s">
+        <v>148</v>
+      </c>
+      <c r="T78" t="b">
+        <v>1</v>
+      </c>
+      <c r="W78" t="s">
+        <v>559</v>
+      </c>
+      <c r="Y78" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB78" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD78" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE78" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH78" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="AI78" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ78" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="AL78" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>560</v>
+      </c>
+      <c r="B79" t="s">
+        <v>563</v>
+      </c>
+      <c r="C79" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79" t="s">
+        <v>36</v>
+      </c>
+      <c r="E79">
+        <v>24.805026282253099</v>
+      </c>
+      <c r="F79">
+        <v>68.605046445490302</v>
+      </c>
+      <c r="G79" s="2">
+        <v>45047</v>
+      </c>
+      <c r="I79" t="s">
+        <v>564</v>
+      </c>
+      <c r="J79" t="s">
+        <v>163</v>
+      </c>
+      <c r="O79" t="s">
+        <v>163</v>
+      </c>
+      <c r="P79" t="s">
+        <v>148</v>
+      </c>
+      <c r="R79" t="b">
+        <v>1</v>
+      </c>
+      <c r="S79" t="b">
+        <v>1</v>
+      </c>
+      <c r="T79" t="b">
+        <v>1</v>
+      </c>
+      <c r="W79" t="s">
+        <v>565</v>
+      </c>
+      <c r="Y79" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB79" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD79" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH79" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="AI79" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ79" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="AL79" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>566</v>
+      </c>
+      <c r="B80" t="s">
+        <v>572</v>
+      </c>
+      <c r="C80" t="s">
+        <v>84</v>
+      </c>
+      <c r="D80" t="s">
+        <v>36</v>
+      </c>
+      <c r="E80">
+        <v>25.506926869862799</v>
+      </c>
+      <c r="F80">
+        <v>69.014789570376706</v>
+      </c>
+      <c r="G80" s="2">
+        <v>45062</v>
+      </c>
+      <c r="I80" t="s">
+        <v>571</v>
+      </c>
+      <c r="J80" t="s">
+        <v>75</v>
+      </c>
+      <c r="O80" t="s">
+        <v>75</v>
+      </c>
+      <c r="P80" t="s">
+        <v>148</v>
+      </c>
+      <c r="W80" t="s">
+        <v>569</v>
+      </c>
+      <c r="Y80" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA80" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="AB80" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC80" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD80" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH80" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="AI80" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ80" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="AL80" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:38" ht="85" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>573</v>
+      </c>
+      <c r="B81" t="s">
+        <v>574</v>
+      </c>
+      <c r="C81" t="s">
+        <v>161</v>
+      </c>
+      <c r="D81" t="s">
+        <v>36</v>
+      </c>
+      <c r="E81">
+        <v>24.8858632112047</v>
+      </c>
+      <c r="F81">
+        <v>67.016539957141106</v>
+      </c>
+      <c r="G81" s="2">
+        <v>45053</v>
+      </c>
+      <c r="H81" t="s">
+        <v>576</v>
+      </c>
+      <c r="I81" t="s">
+        <v>577</v>
+      </c>
+      <c r="J81" t="s">
+        <v>575</v>
+      </c>
+      <c r="O81" t="s">
+        <v>33</v>
+      </c>
+      <c r="P81" t="s">
+        <v>148</v>
+      </c>
+      <c r="R81" t="b">
+        <v>0</v>
+      </c>
+      <c r="S81" t="b">
+        <v>0</v>
+      </c>
+      <c r="T81" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y81" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD81" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH81" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="AI81" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ81" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="AK81" t="s">
+        <v>578</v>
+      </c>
+      <c r="AL81" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:38" ht="68" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>579</v>
+      </c>
+      <c r="B82" t="s">
+        <v>574</v>
+      </c>
+      <c r="C82" t="s">
+        <v>161</v>
+      </c>
+      <c r="D82" t="s">
+        <v>36</v>
+      </c>
+      <c r="E82">
+        <v>24.8858632112047</v>
+      </c>
+      <c r="F82">
+        <v>67.016539957141106</v>
+      </c>
+      <c r="G82" s="2">
+        <v>45053</v>
+      </c>
+      <c r="I82" t="s">
+        <v>580</v>
+      </c>
+      <c r="J82" t="s">
+        <v>581</v>
+      </c>
+      <c r="M82">
+        <v>14</v>
+      </c>
+      <c r="O82" t="s">
+        <v>33</v>
+      </c>
+      <c r="P82" t="s">
+        <v>148</v>
+      </c>
+      <c r="R82" t="b">
+        <v>1</v>
+      </c>
+      <c r="T82" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y82" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD82" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH82" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="AI82" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ82" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="AK82" t="s">
+        <v>588</v>
+      </c>
+      <c r="AL82" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:38" ht="68" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>586</v>
+      </c>
+      <c r="B83" t="s">
+        <v>574</v>
+      </c>
+      <c r="C83" t="s">
+        <v>161</v>
+      </c>
+      <c r="D83" t="s">
+        <v>36</v>
+      </c>
+      <c r="E83">
+        <v>24.8858632112047</v>
+      </c>
+      <c r="F83">
+        <v>67.016539957141106</v>
+      </c>
+      <c r="G83" s="2">
+        <v>45053</v>
+      </c>
+      <c r="I83" t="s">
+        <v>587</v>
+      </c>
+      <c r="J83" t="s">
+        <v>581</v>
+      </c>
+      <c r="M83">
+        <v>12</v>
+      </c>
+      <c r="O83" t="s">
+        <v>33</v>
+      </c>
+      <c r="P83" t="s">
+        <v>148</v>
+      </c>
+      <c r="R83" t="b">
+        <v>1</v>
+      </c>
+      <c r="T83" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y83" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD83" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH83" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="AI83" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ83" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="AK83" t="s">
+        <v>588</v>
+      </c>
+      <c r="AL83" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>589</v>
+      </c>
+      <c r="B84" t="s">
+        <v>53</v>
+      </c>
+      <c r="C84" t="s">
+        <v>53</v>
+      </c>
+      <c r="D84" t="s">
+        <v>36</v>
+      </c>
+      <c r="E84">
+        <v>26.043720730451401</v>
+      </c>
+      <c r="F84">
+        <v>68.947643411108999</v>
+      </c>
+      <c r="G84" s="2">
+        <v>45058</v>
+      </c>
+      <c r="I84" t="s">
+        <v>590</v>
+      </c>
+      <c r="J84" t="s">
+        <v>591</v>
+      </c>
+      <c r="O84" t="s">
+        <v>33</v>
+      </c>
+      <c r="P84" t="s">
+        <v>148</v>
+      </c>
+      <c r="T84" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y84" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD84" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH84" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="AI84" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ84" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="AL84" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:38" ht="85" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>596</v>
+      </c>
+      <c r="B85" t="s">
+        <v>597</v>
+      </c>
+      <c r="C85" t="s">
+        <v>598</v>
+      </c>
+      <c r="D85" t="s">
+        <v>36</v>
+      </c>
+      <c r="E85">
+        <v>25.3497190987339</v>
+      </c>
+      <c r="F85">
+        <v>68.275171571302593</v>
+      </c>
+      <c r="G85" s="2">
+        <v>45054</v>
+      </c>
+      <c r="I85" t="s">
+        <v>599</v>
+      </c>
+      <c r="J85" t="s">
+        <v>600</v>
+      </c>
+      <c r="O85" t="s">
+        <v>33</v>
+      </c>
+      <c r="P85" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD85" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH85" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="AI85" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ85" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="AL85" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>602</v>
+      </c>
+      <c r="B86" t="s">
+        <v>607</v>
+      </c>
+      <c r="C86" t="s">
+        <v>161</v>
+      </c>
+      <c r="D86" t="s">
+        <v>36</v>
+      </c>
+      <c r="E86">
+        <v>24.8619403009107</v>
+      </c>
+      <c r="F86">
+        <v>66.989857731213306</v>
+      </c>
+      <c r="G86" s="2">
+        <v>45051</v>
+      </c>
+      <c r="I86" t="s">
+        <v>605</v>
+      </c>
+      <c r="J86" t="s">
+        <v>606</v>
+      </c>
+      <c r="O86" t="s">
+        <v>163</v>
+      </c>
+      <c r="P86" t="s">
+        <v>145</v>
+      </c>
+      <c r="W86" t="s">
+        <v>601</v>
+      </c>
+      <c r="AD86" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH86" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="AI86" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ86" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="AL86" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>608</v>
+      </c>
+      <c r="B87" t="s">
+        <v>550</v>
+      </c>
+      <c r="C87" t="s">
+        <v>543</v>
+      </c>
+      <c r="D87" t="s">
+        <v>36</v>
+      </c>
+      <c r="E87">
+        <v>28.0389423129139</v>
+      </c>
+      <c r="F87">
+        <v>69.680403992567904</v>
+      </c>
+      <c r="G87" s="2">
+        <v>45043</v>
+      </c>
+      <c r="H87" t="s">
+        <v>615</v>
+      </c>
+      <c r="I87" t="s">
+        <v>609</v>
+      </c>
+      <c r="J87" t="s">
+        <v>610</v>
+      </c>
+      <c r="K87" t="s">
+        <v>613</v>
+      </c>
+      <c r="L87" t="s">
+        <v>485</v>
+      </c>
+      <c r="N87">
+        <v>25</v>
+      </c>
+      <c r="O87" t="s">
+        <v>75</v>
+      </c>
+      <c r="P87" t="s">
+        <v>148</v>
+      </c>
+      <c r="T87" t="b">
+        <v>1</v>
+      </c>
+      <c r="W87" t="s">
+        <v>614</v>
+      </c>
+      <c r="Y87" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z87" t="s">
+        <v>508</v>
+      </c>
+      <c r="AB87" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD87" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH87" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="AI87" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ87" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="AL87" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>616</v>
+      </c>
+      <c r="B88" t="s">
+        <v>620</v>
+      </c>
+      <c r="C88" t="s">
+        <v>53</v>
+      </c>
+      <c r="D88" t="s">
+        <v>36</v>
+      </c>
+      <c r="E88">
+        <v>25.708638069404401</v>
+      </c>
+      <c r="F88">
+        <v>69.128214440080299</v>
+      </c>
+      <c r="G88" s="2">
+        <v>45050</v>
+      </c>
+      <c r="I88" t="s">
+        <v>32</v>
+      </c>
+      <c r="J88" t="s">
+        <v>619</v>
+      </c>
+      <c r="K88" t="s">
+        <v>484</v>
+      </c>
+      <c r="L88" t="s">
+        <v>485</v>
+      </c>
+      <c r="O88" t="s">
+        <v>624</v>
+      </c>
+      <c r="P88" t="s">
+        <v>148</v>
+      </c>
+      <c r="T88" t="b">
+        <v>1</v>
+      </c>
+      <c r="W88" t="s">
+        <v>623</v>
+      </c>
+      <c r="Y88" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z88" t="s">
+        <v>622</v>
+      </c>
+      <c r="AA88" t="s">
+        <v>621</v>
+      </c>
+      <c r="AB88" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD88" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH88" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="AI88" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ88" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="AL88" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:38" ht="85" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>625</v>
+      </c>
+      <c r="B89" t="s">
+        <v>89</v>
+      </c>
+      <c r="C89" t="s">
+        <v>39</v>
+      </c>
+      <c r="D89" t="s">
+        <v>36</v>
+      </c>
+      <c r="E89">
+        <v>25.2842319888404</v>
+      </c>
+      <c r="F89">
+        <v>69.393353732141904</v>
+      </c>
+      <c r="G89" s="2">
+        <v>45047</v>
+      </c>
+      <c r="I89" t="s">
+        <v>149</v>
+      </c>
+      <c r="J89" t="s">
+        <v>628</v>
+      </c>
+      <c r="K89" t="s">
+        <v>630</v>
+      </c>
+      <c r="M89">
+        <v>16</v>
+      </c>
+      <c r="O89" t="s">
+        <v>627</v>
+      </c>
+      <c r="P89" t="s">
+        <v>148</v>
+      </c>
+      <c r="R89" t="b">
+        <v>1</v>
+      </c>
+      <c r="T89" t="b">
+        <v>1</v>
+      </c>
+      <c r="W89" t="s">
+        <v>629</v>
+      </c>
+      <c r="Y89" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB89" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD89" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH89" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="AI89" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ89" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="AL89" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>631</v>
+      </c>
+      <c r="B90" t="s">
+        <v>637</v>
+      </c>
+      <c r="C90" t="s">
+        <v>53</v>
+      </c>
+      <c r="D90" t="s">
+        <v>36</v>
+      </c>
+      <c r="E90">
+        <v>25.957355271358502</v>
+      </c>
+      <c r="F90">
+        <v>68.899901277480495</v>
+      </c>
+      <c r="G90" s="2">
+        <v>45047</v>
+      </c>
+      <c r="I90" t="s">
+        <v>635</v>
+      </c>
+      <c r="J90" t="s">
+        <v>636</v>
+      </c>
+      <c r="O90" t="s">
+        <v>75</v>
+      </c>
+      <c r="P90" t="s">
+        <v>148</v>
+      </c>
+      <c r="R90" t="b">
+        <v>0</v>
+      </c>
+      <c r="T90" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y90" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD90" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE90" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH90" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AI90" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ90" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="AL90" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91" spans="1:38" ht="85" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>638</v>
+      </c>
+      <c r="B91" t="s">
+        <v>641</v>
+      </c>
+      <c r="C91" t="s">
+        <v>161</v>
+      </c>
+      <c r="D91" t="s">
+        <v>36</v>
+      </c>
+      <c r="E91">
+        <v>24.865590617612899</v>
+      </c>
+      <c r="F91">
+        <v>67.000666654225299</v>
+      </c>
+      <c r="G91" s="2">
+        <v>45031</v>
+      </c>
+      <c r="I91" t="s">
+        <v>642</v>
+      </c>
+      <c r="J91" t="s">
+        <v>643</v>
+      </c>
+      <c r="M91">
+        <v>17</v>
+      </c>
+      <c r="N91">
+        <v>17</v>
+      </c>
+      <c r="O91" t="s">
+        <v>163</v>
+      </c>
+      <c r="P91" t="s">
+        <v>148</v>
+      </c>
+      <c r="R91" t="b">
+        <v>1</v>
+      </c>
+      <c r="S91" t="b">
+        <v>1</v>
+      </c>
+      <c r="T91" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y91" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD91" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH91" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="AI91" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ91" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="AL91" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="92" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>646</v>
+      </c>
+      <c r="B92" t="s">
+        <v>647</v>
+      </c>
+      <c r="C92" t="s">
+        <v>35</v>
+      </c>
+      <c r="D92" t="s">
+        <v>36</v>
+      </c>
+      <c r="E92">
+        <v>25.124166742391601</v>
+      </c>
+      <c r="F92">
+        <v>68.891285334593704</v>
+      </c>
+      <c r="G92" s="2">
+        <v>45044</v>
+      </c>
+      <c r="I92" t="s">
+        <v>648</v>
+      </c>
+      <c r="J92" t="s">
+        <v>650</v>
+      </c>
+      <c r="K92" t="s">
+        <v>377</v>
+      </c>
+      <c r="L92" t="s">
+        <v>649</v>
+      </c>
+      <c r="N92">
+        <v>22</v>
+      </c>
+      <c r="O92" t="s">
+        <v>56</v>
+      </c>
+      <c r="P92" t="s">
+        <v>148</v>
+      </c>
+      <c r="S92" t="b">
+        <v>0</v>
+      </c>
+      <c r="T92" t="b">
+        <v>1</v>
+      </c>
+      <c r="W92" t="s">
+        <v>651</v>
+      </c>
+      <c r="X92" t="s">
+        <v>652</v>
+      </c>
+      <c r="Y92" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z92" t="s">
+        <v>570</v>
+      </c>
+      <c r="AB92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD92" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH92" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="AI92" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ92" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="AL92" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:38" ht="85" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>653</v>
+      </c>
+      <c r="B93" t="s">
+        <v>335</v>
+      </c>
+      <c r="C93" t="s">
+        <v>72</v>
+      </c>
+      <c r="D93" t="s">
+        <v>36</v>
+      </c>
+      <c r="E93">
+        <v>24.744765889774701</v>
+      </c>
+      <c r="F93">
+        <v>69.805283959458194</v>
+      </c>
+      <c r="G93" s="2">
+        <v>45037</v>
+      </c>
+      <c r="I93" t="s">
+        <v>656</v>
+      </c>
+      <c r="J93" t="s">
+        <v>56</v>
+      </c>
+      <c r="O93" t="s">
+        <v>56</v>
+      </c>
+      <c r="P93" t="s">
+        <v>657</v>
+      </c>
+      <c r="S93" t="b">
+        <v>1</v>
+      </c>
+      <c r="T93" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD93" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH93" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="AI93" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ93" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="AL93" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="94" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>658</v>
+      </c>
+      <c r="B94" t="s">
+        <v>661</v>
+      </c>
+      <c r="C94" t="s">
+        <v>543</v>
+      </c>
+      <c r="D94" t="s">
+        <v>36</v>
+      </c>
+      <c r="E94">
+        <v>27.8440081598979</v>
+      </c>
+      <c r="F94">
+        <v>69.414288955958995</v>
+      </c>
+      <c r="G94" s="2">
+        <v>45040</v>
+      </c>
+      <c r="I94" t="s">
+        <v>662</v>
+      </c>
+      <c r="J94" t="s">
+        <v>33</v>
+      </c>
+      <c r="O94" t="s">
+        <v>33</v>
+      </c>
+      <c r="P94" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q94" t="s">
+        <v>663</v>
+      </c>
+      <c r="T94" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB94" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD94" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH94" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="AI94" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ94" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="AL94" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:38" ht="102" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>664</v>
+      </c>
+      <c r="B95" t="s">
+        <v>637</v>
+      </c>
+      <c r="C95" t="s">
+        <v>53</v>
+      </c>
+      <c r="D95" t="s">
+        <v>36</v>
+      </c>
+      <c r="E95">
+        <v>25.957585848306</v>
+      </c>
+      <c r="F95">
+        <v>68.899858074783097</v>
+      </c>
+      <c r="G95" s="2">
+        <v>45036</v>
+      </c>
+      <c r="I95" t="s">
+        <v>668</v>
+      </c>
+      <c r="J95" t="s">
+        <v>668</v>
+      </c>
+      <c r="K95" t="s">
+        <v>667</v>
+      </c>
+      <c r="P95" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>669</v>
+      </c>
+      <c r="T95" t="b">
+        <v>1</v>
+      </c>
+      <c r="W95" t="s">
+        <v>670</v>
+      </c>
+      <c r="Y95" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH95" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="AI95" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ95" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="AL95" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AL73" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}"/>
+  <autoFilter ref="A1:AL93" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}"/>
   <hyperlinks>
     <hyperlink ref="AJ3" r:id="rId1" display="https://twitter.com/NarainDasBheel8/status/1620065868813328387?s=20&amp;t=Ltd0v4nT-kPYw66t6kNWdQ" xr:uid="{7D36CF03-D602-604F-9081-06B44641DFED}"/>
     <hyperlink ref="AJ4" r:id="rId2" xr:uid="{BACCB937-A5FB-A547-AC6D-BEE6543D6916}"/>
@@ -6977,6 +8791,27 @@
     <hyperlink ref="AJ71" r:id="rId89" xr:uid="{B0216B79-0468-2D41-92BF-3C82914A10DF}"/>
     <hyperlink ref="AJ73" r:id="rId90" xr:uid="{5940FE61-4D36-F740-8EA4-FF0BF0B77607}"/>
     <hyperlink ref="AJ74" r:id="rId91" xr:uid="{F850490C-9ED2-A84E-8070-C7A5FCC211DA}"/>
+    <hyperlink ref="AJ75" r:id="rId92" xr:uid="{6BDB9790-FD26-4D41-A106-3C7C6F3988DB}"/>
+    <hyperlink ref="AJ76" r:id="rId93" xr:uid="{AACE243D-6C85-6846-B043-6504F9FFB186}"/>
+    <hyperlink ref="AJ77" r:id="rId94" xr:uid="{84A4A856-EEDF-F544-AB1B-EC545161E0E2}"/>
+    <hyperlink ref="AJ78" r:id="rId95" xr:uid="{64B3A3F7-EF2C-7E41-BCAB-C81070AA386A}"/>
+    <hyperlink ref="AJ79" r:id="rId96" xr:uid="{0EA01EE8-3788-B14F-8981-AC25C7530375}"/>
+    <hyperlink ref="AJ80" r:id="rId97" xr:uid="{A0D1A6D3-CB4D-9947-AB5C-0795C9734323}"/>
+    <hyperlink ref="AJ81" r:id="rId98" xr:uid="{9E16C8D2-482E-E641-B629-3B281A2B176F}"/>
+    <hyperlink ref="AJ82" r:id="rId99" xr:uid="{D203862B-EB55-B74A-B762-57DAFBAA9D35}"/>
+    <hyperlink ref="AJ83" r:id="rId100" xr:uid="{CBCC7836-256D-1F44-AF55-8AE15C15B2D8}"/>
+    <hyperlink ref="AJ84" r:id="rId101" xr:uid="{3A6CB738-EDFE-7949-895D-51A2CBB498A2}"/>
+    <hyperlink ref="AJ85" r:id="rId102" xr:uid="{2AE63782-04E1-F843-8B77-DC5921608932}"/>
+    <hyperlink ref="AJ86" r:id="rId103" xr:uid="{94A09300-0A22-4542-8B49-039987568A7F}"/>
+    <hyperlink ref="AJ87" r:id="rId104" xr:uid="{A83F027B-0ACC-7E47-B96F-176BFBA656C8}"/>
+    <hyperlink ref="AJ88" r:id="rId105" xr:uid="{12425F19-FD98-7544-B45C-08577EABC483}"/>
+    <hyperlink ref="AJ89" r:id="rId106" xr:uid="{CB5D1E8F-408D-1541-AA99-ED89C69AAB8B}"/>
+    <hyperlink ref="AJ90" r:id="rId107" xr:uid="{442CFEF9-53D7-4F43-98E9-2F2ACB01550D}"/>
+    <hyperlink ref="AJ91" r:id="rId108" xr:uid="{82346E6E-4C6A-7A47-BBDE-607E8279831C}"/>
+    <hyperlink ref="AJ92" r:id="rId109" xr:uid="{343F6CD9-A3A4-9449-99AE-03A0FF2FF4BE}"/>
+    <hyperlink ref="AJ93" r:id="rId110" xr:uid="{22900142-D326-6E4A-9EF3-E78B11E3C4DF}"/>
+    <hyperlink ref="AJ94" r:id="rId111" xr:uid="{1AAFEBDA-B464-2C4F-B7F8-F6E93BC43DEB}"/>
+    <hyperlink ref="AJ95" r:id="rId112" xr:uid="{0ED21344-B267-7542-B6E6-35CB137D6861}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
correction for case 9, added asset files
</commit_message>
<xml_diff>
--- a/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
+++ b/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Janak_Jain/Janak/Personal/projects/hindus_in_pakistan/github/hindus_in_pakistan/data/daahip-w/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98A062F-64D7-014B-9F7F-0743CEB6D058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A2A4BA-E148-8E47-9D81-D99D6CED35E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{7834C0CA-90C6-1E41-85BA-104BC8C7D625}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" xr2:uid="{7834C0CA-90C6-1E41-85BA-104BC8C7D625}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -2798,9 +2798,9 @@
   <dimension ref="A1:AL101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3428,7 +3428,7 @@
         <v>69.563337765019099</v>
       </c>
       <c r="G10" s="2">
-        <v>45285</v>
+        <v>44950</v>
       </c>
       <c r="I10" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
added new cases + updated temple list
</commit_message>
<xml_diff>
--- a/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
+++ b/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Janak_Jain/Janak/Personal/projects/hindus_in_pakistan/github/hindus_in_pakistan/data/daahip-w/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B731064D-302B-0D49-B348-A0C41AEC7589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484670EE-98C4-794B-8EE0-5A872357011B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" xr2:uid="{7834C0CA-90C6-1E41-85BA-104BC8C7D625}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="762">
   <si>
     <t>city</t>
   </si>
@@ -2543,6 +2543,25 @@
   </si>
   <si>
     <t>Lachhmi</t>
+  </si>
+  <si>
+    <t>case_107</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1666682798126649346</t>
+  </si>
+  <si>
+    <t>Village Bhader Jalbani near Chambar town</t>
+  </si>
+  <si>
+    <t>Raveena</t>
+  </si>
+  <si>
+    <t>Jumoon Pathan, Akhtar Pathan</t>
+  </si>
+  <si>
+    <t>Tando Allahyar, Sindh
+A Minor Hindu girl Raveena Meghwar, 15, of village Bhader Jalbani near Chambar town, was abducted at gunpoint by Jumoon Pathan and Akhtar Pathan. FIR has been filed against kidnappers. While her school leaving certificate proves Raveena was born on April 18, 2008 making her a minor, the conversion certificate fabricated an age of 22 to claim she is an adult.</t>
   </si>
 </sst>
 </file>
@@ -2961,12 +2980,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}">
-  <dimension ref="A1:AM107"/>
+  <dimension ref="A1:AM108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7450,7 +7469,7 @@
         <v>43880</v>
       </c>
       <c r="H67" s="10">
-        <f t="shared" ref="H67:H107" si="1">WEEKDAY(G67)</f>
+        <f t="shared" ref="H67:H108" si="1">WEEKDAY(G67)</f>
         <v>4</v>
       </c>
       <c r="I67" s="3" t="s">
@@ -10329,6 +10348,90 @@
       </c>
       <c r="AM107" s="3" t="s">
         <v>746</v>
+      </c>
+    </row>
+    <row r="108" spans="1:39" ht="85" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E108" s="3">
+        <v>25.292684680917802</v>
+      </c>
+      <c r="F108" s="3">
+        <v>68.818482632061205</v>
+      </c>
+      <c r="G108" s="4">
+        <v>45056</v>
+      </c>
+      <c r="H108" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J108" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="K108" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L108" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="N108" s="3">
+        <v>15</v>
+      </c>
+      <c r="O108" s="3">
+        <v>22</v>
+      </c>
+      <c r="P108" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q108" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="S108" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T108" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="U108" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="X108" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="Z108" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC108" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE108" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF108" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI108" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="AJ108" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK108" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="AM108" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -10459,6 +10562,7 @@
     <hyperlink ref="AK105" r:id="rId123" xr:uid="{161FE759-E448-A749-A840-BE3DB023CD43}"/>
     <hyperlink ref="AK106" r:id="rId124" xr:uid="{DC0D86EB-1BD6-8D42-A44A-B4CCBF588BBA}"/>
     <hyperlink ref="AK107" r:id="rId125" xr:uid="{8E848CC0-3E3C-864E-B797-D778F447BD8C}"/>
+    <hyperlink ref="AK108" r:id="rId126" xr:uid="{CC1936A8-EB33-8247-A5FD-9AA49D3877FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
added new case + updated temple dataset
</commit_message>
<xml_diff>
--- a/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
+++ b/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Janak_Jain/Janak/Personal/projects/hindus_in_pakistan/github/hindus_in_pakistan/data/daahip-w/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368415E8-74A4-DD41-BB6B-7DE5FF8B0623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDA3134-D580-4E41-B331-372891A96929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" xr2:uid="{7834C0CA-90C6-1E41-85BA-104BC8C7D625}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="cases" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cases!$A$1:$AM$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cases!$A$1:$AM$113</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="795">
   <si>
     <t>city</t>
   </si>
@@ -2656,6 +2656,22 @@
   </si>
   <si>
     <t>44402-4840647-9</t>
+  </si>
+  <si>
+    <t>case_113</t>
+  </si>
+  <si>
+    <t>Sukkur Sindh:
+A few days ago, a Hindu girl, Riya Kumari, was abducted from Sukkur, converted to Islam and  married to Muhammad Raza Qureshi.</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1679864614962577410</t>
+  </si>
+  <si>
+    <t>Riya</t>
+  </si>
+  <si>
+    <t>Muhammad Raza Qureshi</t>
   </si>
 </sst>
 </file>
@@ -3074,12 +3090,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}">
-  <dimension ref="A1:AM113"/>
+  <dimension ref="A1:AM114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A113" sqref="A113"/>
+      <selection pane="bottomLeft" activeCell="AJ114" sqref="AJ114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7563,7 +7579,7 @@
         <v>43880</v>
       </c>
       <c r="H67" s="10">
-        <f t="shared" ref="H67:H113" si="1">WEEKDAY(G67)</f>
+        <f t="shared" ref="H67:H114" si="1">WEEKDAY(G67)</f>
         <v>4</v>
       </c>
       <c r="I67" s="3" t="s">
@@ -10870,8 +10886,71 @@
         <v>24</v>
       </c>
     </row>
+    <row r="114" spans="1:39" ht="51" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E114" s="3">
+        <v>27.725658113185499</v>
+      </c>
+      <c r="F114" s="3">
+        <v>68.821808554497906</v>
+      </c>
+      <c r="G114" s="4">
+        <v>45121</v>
+      </c>
+      <c r="H114" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="K114" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q114" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="U114" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="X114" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="Z114" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC114" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE114" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI114" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="AJ114" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK114" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="AM114" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AM108" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}"/>
+  <autoFilter ref="A1:AM113" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}"/>
   <hyperlinks>
     <hyperlink ref="AK3" r:id="rId1" display="https://twitter.com/NarainDasBheel8/status/1620065868813328387?s=20&amp;t=Ltd0v4nT-kPYw66t6kNWdQ" xr:uid="{7D36CF03-D602-604F-9081-06B44641DFED}"/>
     <hyperlink ref="AK4" r:id="rId2" xr:uid="{BACCB937-A5FB-A547-AC6D-BEE6543D6916}"/>
@@ -11004,6 +11083,7 @@
     <hyperlink ref="AK111" r:id="rId129" xr:uid="{DF57C7D5-1DB0-CE4A-AD6A-E4A5516A077C}"/>
     <hyperlink ref="AK112" r:id="rId130" xr:uid="{FAE47F1D-22DE-824F-9ECC-F63DEB17631A}"/>
     <hyperlink ref="AK113" r:id="rId131" xr:uid="{04F7AEA5-DEBF-CD4D-943E-BDA0F8DC4729}"/>
+    <hyperlink ref="AK114" r:id="rId132" xr:uid="{8091E0DF-5902-9840-BA05-BCDCC81E6506}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added new case + updated README
</commit_message>
<xml_diff>
--- a/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
+++ b/data/daahip-w/20230131_list_violence_abductions_forced_conversions_hindu_women_in_pakistan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Janak_Jain/Janak/Personal/projects/hindus_in_pakistan/github/hindus_in_pakistan/data/daahip-w/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BC5F81-3BA7-2C4E-82A8-4ABF0EBBC209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6788CB1-1C8F-7441-B838-20F15C62A38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" xr2:uid="{7834C0CA-90C6-1E41-85BA-104BC8C7D625}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="812">
   <si>
     <t>city</t>
   </si>
@@ -2714,6 +2714,20 @@
 A few days ago, the kidnapped Hindu girl #Meena_Kolhi reached her home. She says that after she was abducted and forcefully converted to islam, she was married to Iqbal Bhambhro was r@ped by many people.
 #StopForcedConversions
 #saveminoritygirls</t>
+  </si>
+  <si>
+    <t>case_116</t>
+  </si>
+  <si>
+    <t>Hyderabad Sindh Pakistan:
+13-year-old Hindu girl Shanti Kolhi from Kohsar, Hyderabad Sindh has been abducted and converted.
+Protest demonstration in front of  Press Club Hyderabad…</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NarainDasBheel8/status/1690315060844130304</t>
+  </si>
+  <si>
+    <t>Kohsar</t>
   </si>
 </sst>
 </file>
@@ -3132,12 +3146,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2FE676-F03D-4E4C-8907-AA9304B213EE}">
-  <dimension ref="A1:AM116"/>
+  <dimension ref="A1:AM117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="AK47" sqref="AK47"/>
+      <selection pane="bottomLeft" activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7621,7 +7635,7 @@
         <v>43880</v>
       </c>
       <c r="H67" s="10">
-        <f t="shared" ref="H67:H116" si="1">WEEKDAY(G67)</f>
+        <f t="shared" ref="H67:H117" si="1">WEEKDAY(G67)</f>
         <v>4</v>
       </c>
       <c r="I67" s="3" t="s">
@@ -11147,6 +11161,72 @@
         <v>806</v>
       </c>
       <c r="AM116" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:39" ht="68" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E117" s="3">
+        <v>25.3341223610492</v>
+      </c>
+      <c r="F117" s="3">
+        <v>68.364220234733594</v>
+      </c>
+      <c r="G117" s="4">
+        <v>45149</v>
+      </c>
+      <c r="H117" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J117" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="K117" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="N117" s="3">
+        <v>13</v>
+      </c>
+      <c r="P117" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q117" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="S117" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U117" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z117" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE117" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI117" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="AJ117" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK117" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="AM117" s="3" t="s">
         <v>24</v>
       </c>
     </row>
@@ -11287,6 +11367,7 @@
     <hyperlink ref="AK114" r:id="rId132" xr:uid="{8091E0DF-5902-9840-BA05-BCDCC81E6506}"/>
     <hyperlink ref="AK115" r:id="rId133" xr:uid="{EF492A6F-E433-264C-88E7-58575B339902}"/>
     <hyperlink ref="AK116" r:id="rId134" xr:uid="{CDCC03B3-84C4-334F-AEB9-9A785AFD1877}"/>
+    <hyperlink ref="AK117" r:id="rId135" xr:uid="{FA5FA8CD-C223-4A4D-A19C-B2EA358D5CFA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>